<commit_message>
Working target and adj algorithms. All tests pass 100%.
</commit_message>
<xml_diff>
--- a/data/ClueLayout306.xlsx
+++ b/data/ClueLayout306.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanga/Library/Mobile Documents/com~apple~CloudDocs/School/CSCI 306 - Software Engineering/csci306-workspace/ClueGame/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A67C17-64CD-CC4E-BBA0-0F6028AE2814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD268097-9AAD-214C-80BB-131C442C5453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3130,7 +3130,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>